<commit_message>
Report - Quay section near completion
</commit_message>
<xml_diff>
--- a/excel_data/world_population.xlsx
+++ b/excel_data/world_population.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Checkouts\Terminal_optimization\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F111A5CE-D3A9-4A3F-A8ED-5B679ED98F19}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB12493B-BEDA-4FD6-BACF-C4FDDF36A8B2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="11550" firstSheet="7" activeTab="10" xr2:uid="{80943641-C598-4655-A746-ABA473811383}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="11550" activeTab="3" xr2:uid="{80943641-C598-4655-A746-ABA473811383}"/>
   </bookViews>
   <sheets>
     <sheet name="Population vs GDP" sheetId="1" r:id="rId1"/>
@@ -5359,7 +5359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADADF12-7B03-4605-89AF-268E62FDFDE2}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -13849,8 +13849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FD8FEA-28B5-45FA-AA9F-5EED8A3D7CD6}">
   <dimension ref="A1:AC683"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AG29" sqref="AG29"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="X29" sqref="X29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>